<commit_message>
Minor update to Arduino pin mapping for TC4 shields.
</commit_message>
<xml_diff>
--- a/TC4/docs/TC4-pins.xlsx
+++ b/TC4/docs/TC4-pins.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
-  <si>
-    <t>Arduino pin assignments</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Pin</t>
   </si>
@@ -39,9 +36,6 @@
     <t>D4</t>
   </si>
   <si>
-    <t>D5</t>
-  </si>
-  <si>
     <t>Descrip.</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>OT2</t>
   </si>
   <si>
-    <t>PWM/millis()</t>
-  </si>
-  <si>
     <t>A0</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>A5</t>
   </si>
   <si>
-    <t>I2C</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -120,9 +108,6 @@
     <t>INT0</t>
   </si>
   <si>
-    <t>I/O3 &amp; Jee3-6</t>
-  </si>
-  <si>
     <t>Jee3-2</t>
   </si>
   <si>
@@ -157,13 +142,52 @@
   </si>
   <si>
     <t>by the underlying hardware, is not currently included in the Arduino language.</t>
+  </si>
+  <si>
+    <t>Updated 5/12/14</t>
+  </si>
+  <si>
+    <t>IO2</t>
+  </si>
+  <si>
+    <t>IO3 &amp; Jee3-6</t>
+  </si>
+  <si>
+    <t>I2C (SDA)</t>
+  </si>
+  <si>
+    <t>I2C (SCL)</t>
+  </si>
+  <si>
+    <t>Arduino pin descriptions</t>
+  </si>
+  <si>
+    <t>D5**</t>
+  </si>
+  <si>
+    <t>D6**</t>
+  </si>
+  <si>
+    <t>** These pins support PWM provided by timer0.  Timer0 is also used</t>
+  </si>
+  <si>
+    <t>for the millis() and analogWrite() functions.</t>
+  </si>
+  <si>
+    <t>Note:  Many Jee devices are 3.3V</t>
+  </si>
+  <si>
+    <t>and will not be compatible with</t>
+  </si>
+  <si>
+    <t>the 5V signals from Arduino.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +221,12 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -303,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -341,24 +371,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -375,6 +387,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,7 +708,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -688,14 +721,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
@@ -708,26 +743,26 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="13"/>
@@ -737,10 +772,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="13"/>
@@ -750,12 +785,14 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -763,13 +800,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
@@ -778,7 +815,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="12"/>
@@ -789,10 +826,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
@@ -802,67 +839,73 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="16"/>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="16"/>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="37" t="s">
         <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -871,43 +914,43 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>28</v>
+      <c r="D15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E16" s="14">
         <v>1</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="12"/>
@@ -916,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -929,102 +972,96 @@
         <v>3</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14">
         <v>4</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14">
         <v>5</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="34"/>
+        <v>31</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="17">
         <v>6</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="1"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="1"/>
+      <c r="C23" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1"/>
+      <c r="C24" s="38" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="32" t="s">
-        <v>45</v>
-      </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1033,8 +1070,8 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
+      <c r="A26" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1044,7 +1081,9 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -1053,7 +1092,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="16"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="16"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -1062,7 +1101,9 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="16"/>
+      <c r="A29" s="39" t="s">
+        <v>50</v>
+      </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -1071,7 +1112,9 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="16"/>
+      <c r="A30" s="39" t="s">
+        <v>51</v>
+      </c>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>

</xml_diff>